<commit_message>
some data and inital version r script
</commit_message>
<xml_diff>
--- a/analysis/time_avg_and_filter.xlsx
+++ b/analysis/time_avg_and_filter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiaskuehlwein/pm_color/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB166DEB-8C7D-3F43-86D7-091B99A98FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B346B59D-2389-0044-BF7A-88FA43E86B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17760" yWindow="-18720" windowWidth="27240" windowHeight="14800" xr2:uid="{F7A8C53D-62F3-474D-856C-CDF2FED7D69A}"/>
+    <workbookView xWindow="760" yWindow="1980" windowWidth="27240" windowHeight="14800" xr2:uid="{F7A8C53D-62F3-474D-856C-CDF2FED7D69A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13426,8 +13426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC215302-4163-914D-9A92-5509E7663915}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13812,7 +13812,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(B23,FIND("color_offset",B23)+1,FIND(",",B23,FIND("color_offset",B23))-FIND("color_offset",B23)-1)</f>
         <v>olor_offset":-151.77448375144087</v>
       </c>
       <c r="B23" s="1" t="s">

</xml_diff>